<commit_message>
Update Structurizer, Utilizer, main
</commit_message>
<xml_diff>
--- a/cases_with_reasoning_test_withVerdict.xlsx
+++ b/cases_with_reasoning_test_withVerdict.xlsx
@@ -556,32 +556,32 @@
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>涉及共犯？</t>
+          <t>verdict</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>涉及外國人？</t>
+          <t>reason</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>和解？</t>
+          <t>媒體影響_value</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>被害人考量？</t>
+          <t>媒體影響_type</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>verdict</t>
+          <t>量刑爭議_value</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>reason</t>
+          <t>量刑爭議_type</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -749,7 +749,7 @@
         </is>
       </c>
       <c r="T2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" t="b">
         <v>0</v>
@@ -766,24 +766,21 @@
       <c r="Y2" t="b">
         <v>0</v>
       </c>
-      <c r="Z2" t="b">
-        <v>0</v>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>。根據裁定書的理由，法院認為本案存在不適宜行國民參與審判的情事，包括被告已對被訴事實作有罪陳述、案件情節可能對被害人家屬造成二度傷害，以及案件涉及的證據可能對國民法官造成過大刺激，符合國民法官法第6條第1項第4款及第5款的規定。</t>
+        </is>
       </c>
       <c r="AA2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>**結論：FALSE**，法院裁定不行國民參與審判，主要原因是被告已為有罪陳述且被害人家屬明確表示希望不行國民參與審判以避免媒體報導對未成年子女造成二度傷害。
-法院在裁定中明確指出依據國民法官法第6條第1項第4款(被告已為有罪陳述)及第5款(其他有事實足認行國民參與審判顯不適當)，決定不行國民參與審判。布林表中L4和L5為TRUE，且被害人考量也為TRUE，這些都支持法院的裁定結果。法院特別重視被害人家屬(訴訟參與人)的意見，認為國民參與審判可能導致媒體過度報導，對被害人未成年子女造成難以回復的負面影響。</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -939,22 +936,19 @@
       <c r="Y3" t="b">
         <v>0</v>
       </c>
-      <c r="Z3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB3" t="b">
-        <v>1</v>
-      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>。根據裁定書的理由，雖然本案符合國民法官法第5條第1項第2款的適用條件，但被告已認罪且與被害人家屬達成和解，且檢辯雙方對於量刑無重大爭執，因此法院認為不行國民參與審判為適當。</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="b">
         <v>0</v>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>結論
-**FALSE**：法院裁定不行國民參與審判，因為被告已認罪、與被害人家屬達成和解，且被害人家屬同意不進行國民參與審判，符合國民法官法第6條第1項第4款的排除條件。</t>
+          <t>bool</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Structurizer, Utilizer, main, prompts
</commit_message>
<xml_diff>
--- a/cases_with_reasoning_test_withVerdict.xlsx
+++ b/cases_with_reasoning_test_withVerdict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,20 +566,60 @@
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
+          <t>涉及共犯_value</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>涉及共犯_type</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>涉及外國人_value</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>涉及外國人_type</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>和解_value</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>和解_type</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>被害人考量_value</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>被害人考量_type</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
           <t>媒體影響_value</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>媒體影響_type</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>量刑爭議_value</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>量刑爭議_type</t>
         </is>
@@ -626,7 +666,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -768,19 +808,51 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>。根據裁定書的理由，法院認為本案存在不適宜行國民參與審判的情事，包括被告已對被訴事實作有罪陳述、案件情節可能對被害人家屬造成二度傷害，以及案件涉及的證據可能對國民法官造成過大刺激，符合國民法官法第6條第1項第4款及第5款的規定。</t>
+          <t>因為被告已對被訴事實作有罪陳述，且案件情節涉及媒體影響及被害人家屬的意見，法院認為行國民參與審判可能對被害人家屬造成二度傷害，且不適合彰顯國民參與審判的價值。</t>
         </is>
       </c>
       <c r="AA2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
           <t>bool</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
+      <c r="AC2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="AE2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="AG2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="AI2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -925,7 +997,7 @@
         <v>0</v>
       </c>
       <c r="V3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" t="b">
         <v>1</v>
@@ -938,15 +1010,47 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>。根據裁定書的理由，雖然本案符合國民法官法第5條第1項第2款的適用條件，但被告已認罪且與被害人家屬達成和解，且檢辯雙方對於量刑無重大爭執，因此法院認為不行國民參與審判為適當。</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
+          <t>因為被告已對被訴事實為有罪陳述，且檢辯雙方對於量刑無重大爭議，並且被害人家屬已表達同意不進行國民參與審判程序，符合國民法官法第6條第1項第4款的規定。</t>
+        </is>
+      </c>
+      <c r="AA3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
       <c r="AC3" t="b">
         <v>0</v>
       </c>
       <c r="AD3" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="AE3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="AG3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL3" t="inlineStr">
         <is>
           <t>bool</t>
         </is>

</xml_diff>